<commit_message>
fix lab1 and lab2
</commit_message>
<xml_diff>
--- a/docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759C941C-35C0-4E5B-9175-2A1A75B18503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9CBA27-BF65-4BD3-8774-8AB120DF367F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="106">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -340,9 +340,6 @@
     <t>...</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -495,12 +492,6 @@
     <t>intrerval&lt;1</t>
   </si>
   <si>
-    <t>startTime&gt;=1970</t>
-  </si>
-  <si>
-    <t>startTime&lt;1970</t>
-  </si>
-  <si>
     <t>startTime</t>
   </si>
   <si>
@@ -531,12 +522,6 @@
     <t>12.11.1995 12:00</t>
   </si>
   <si>
-    <t>task added</t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>interval&gt;=1</t>
   </si>
   <si>
@@ -598,6 +583,18 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>startTime&lt;=1970</t>
   </si>
 </sst>
 </file>
@@ -1270,7 +1267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1384,6 +1381,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1399,13 +1413,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1435,53 +1488,35 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1495,23 +1530,79 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1525,114 +1616,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1957,12 +1940,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="54"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63"/>
       <c r="H1" s="49" t="s">
         <v>1</v>
       </c>
@@ -1970,11 +1953,11 @@
       <c r="J1" s="49"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H3" s="2"/>
@@ -1990,7 +1973,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="2">
         <v>235</v>
@@ -2001,7 +1984,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J5" s="2">
         <v>235</v>
@@ -2013,7 +1996,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J6" s="2">
         <v>235</v>
@@ -2061,16 +2044,16 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:10" ht="74" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="121" t="s">
-        <v>63</v>
+      <c r="B15" s="51" t="s">
+        <v>62</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="122" t="s">
-        <v>64</v>
+      <c r="B16" s="52" t="s">
+        <v>63</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2093,7 +2076,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C20" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -2137,21 +2120,21 @@
     </row>
     <row r="24" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="46"/>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C26" s="48"/>
@@ -2175,7 +2158,7 @@
   <dimension ref="B1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2196,43 +2179,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B3" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="B3" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="83"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="G5" s="63" t="s">
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="G5" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" s="22" t="s">
@@ -2247,86 +2230,86 @@
       <c r="E6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="78" t="s">
+      <c r="H6" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="76" t="s">
+      <c r="I6" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="80" t="s">
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="80"/>
+      <c r="Q6" s="78"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="125" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="125"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="79"/>
+      <c r="C7" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="77"/>
       <c r="I7" s="22" t="s">
         <v>30</v>
       </c>
       <c r="J7" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="N7" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="L7" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="N7" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="O7" s="77"/>
-      <c r="P7" s="76" t="s">
+      <c r="O7" s="75"/>
+      <c r="P7" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="77"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125" t="s">
-        <v>73</v>
+      <c r="C8" s="66"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="G8" s="22">
         <v>1</v>
       </c>
-      <c r="H8" s="2">
-        <v>1</v>
+      <c r="H8" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L8" s="2" t="b">
         <v>1</v>
@@ -2334,141 +2317,145 @@
       <c r="M8" s="2">
         <v>3</v>
       </c>
-      <c r="N8" s="74" t="b">
+      <c r="N8" s="70" t="b">
         <v>1</v>
       </c>
-      <c r="O8" s="75" t="s">
+      <c r="O8" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="74" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q8" s="75"/>
+      <c r="P8" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="95"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="125" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="125"/>
+      <c r="C9" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="4"/>
       <c r="G9" s="22">
         <v>2</v>
       </c>
-      <c r="H9" s="2">
-        <v>2</v>
+      <c r="H9" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N9" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q9" s="75"/>
+        <v>80</v>
+      </c>
+      <c r="L9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>3</v>
+      </c>
+      <c r="N9" s="70" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="72" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q9" s="73"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125" t="s">
-        <v>71</v>
+      <c r="C10" s="66"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="G10" s="34">
         <v>3</v>
       </c>
-      <c r="H10" s="13">
-        <v>3</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="124" t="s">
-        <v>105</v>
-      </c>
-      <c r="K10" s="124" t="s">
-        <v>81</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>33</v>
+      <c r="H10" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="M10" s="13">
         <v>2</v>
       </c>
-      <c r="N10" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="69"/>
-      <c r="P10" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q10" s="69"/>
+      <c r="N10" s="70" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="95"/>
     </row>
     <row r="11" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="56"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="G11" s="34">
         <v>4</v>
       </c>
-      <c r="H11" s="13">
-        <v>4</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>33</v>
+      <c r="H11" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="M11" s="13">
         <v>-12</v>
       </c>
-      <c r="N11" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="O11" s="69"/>
-      <c r="P11" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q11" s="69"/>
+      <c r="N11" s="70" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="72" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q11" s="73"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="56"/>
+      <c r="C12" s="80"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="G12" s="12">
@@ -2480,16 +2467,16 @@
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="70"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="70"/>
-      <c r="Q12" s="71"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="68"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="G13" s="12">
@@ -2501,16 +2488,16 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="70"/>
-      <c r="O13" s="71"/>
-      <c r="P13" s="70"/>
-      <c r="Q13" s="71"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="68"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="58"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="G14" s="18">
@@ -2522,8 +2509,8 @@
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="67"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="89"/>
       <c r="P14" s="72"/>
       <c r="Q14" s="73"/>
     </row>
@@ -2531,7 +2518,7 @@
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="80" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="4"/>
@@ -2545,8 +2532,8 @@
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="75"/>
+      <c r="N15" s="70"/>
+      <c r="O15" s="71"/>
       <c r="P15" s="72"/>
       <c r="Q15" s="73"/>
     </row>
@@ -2554,7 +2541,7 @@
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="56"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="18"/>
@@ -2564,8 +2551,8 @@
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="75"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="71"/>
       <c r="P16" s="72"/>
       <c r="Q16" s="73"/>
     </row>
@@ -2573,7 +2560,7 @@
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="80" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="4"/>
@@ -2585,8 +2572,8 @@
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="75"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="71"/>
       <c r="P17" s="72"/>
       <c r="Q17" s="73"/>
     </row>
@@ -2594,7 +2581,7 @@
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="56"/>
+      <c r="C18" s="80"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="18"/>
@@ -2604,8 +2591,8 @@
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="74"/>
-      <c r="O18" s="75"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="71"/>
       <c r="P18" s="72"/>
       <c r="Q18" s="73"/>
     </row>
@@ -2613,7 +2600,7 @@
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="80" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="4"/>
@@ -2625,8 +2612,8 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="74"/>
-      <c r="O19" s="75"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="71"/>
       <c r="P19" s="72"/>
       <c r="Q19" s="73"/>
     </row>
@@ -2634,32 +2621,33 @@
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="56"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
+        <v>35</v>
+      </c>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="P9:Q9"/>
@@ -2675,20 +2663,19 @@
     <mergeCell ref="N13:O13"/>
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="N11:O11"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2702,7 +2689,7 @@
   <dimension ref="B1:R30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="Q9" sqref="Q9:R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2725,122 +2712,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="83"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="63"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="85"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="I6" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="J6" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="78" t="s">
+      <c r="K6" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="99"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B7" s="65">
+        <v>1</v>
+      </c>
+      <c r="C7" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="64">
+        <v>0</v>
+      </c>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q7" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="134" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="136"/>
-      <c r="Q6" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="91"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B7" s="57">
-        <v>1</v>
-      </c>
-      <c r="C7" s="84" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="55">
-        <v>0</v>
-      </c>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="126" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="126" t="s">
-        <v>74</v>
-      </c>
-      <c r="M7" s="126" t="s">
-        <v>75</v>
-      </c>
-      <c r="N7" s="126" t="s">
-        <v>76</v>
-      </c>
-      <c r="O7" s="126" t="s">
-        <v>77</v>
-      </c>
-      <c r="P7" s="126" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q7" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="R7" s="77"/>
+      <c r="R7" s="75"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B8" s="83"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="55"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="64"/>
       <c r="G8" s="18">
         <v>1</v>
       </c>
@@ -2848,19 +2835,19 @@
         <v>1</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="N8" s="17" t="b">
         <v>1</v>
@@ -2872,19 +2859,19 @@
         <v>1</v>
       </c>
       <c r="Q8" s="72" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="R8" s="73"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B9" s="83">
+      <c r="B9" s="93">
         <v>2</v>
       </c>
-      <c r="C9" s="85"/>
-      <c r="D9" s="55">
+      <c r="C9" s="101"/>
+      <c r="D9" s="64">
         <v>1</v>
       </c>
-      <c r="G9" s="130">
+      <c r="G9" s="53">
         <v>2</v>
       </c>
       <c r="H9" s="16">
@@ -2894,7 +2881,7 @@
         <v>33</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K9" s="32" t="s">
         <v>33</v>
@@ -2914,16 +2901,16 @@
       <c r="P9" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="92" t="s">
-        <v>95</v>
-      </c>
-      <c r="R9" s="93"/>
+      <c r="Q9" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="R9" s="95"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B10" s="83"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="55"/>
-      <c r="G10" s="130">
+      <c r="B10" s="93"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="64"/>
+      <c r="G10" s="53">
         <v>3</v>
       </c>
       <c r="H10" s="16">
@@ -2933,7 +2920,7 @@
         <v>33</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K10" s="32" t="s">
         <v>33</v>
@@ -2953,17 +2940,17 @@
       <c r="P10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="92" t="s">
-        <v>95</v>
-      </c>
-      <c r="R10" s="93"/>
+      <c r="Q10" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="R10" s="95"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B11" s="83">
+      <c r="B11" s="93">
         <v>3</v>
       </c>
-      <c r="C11" s="85"/>
-      <c r="D11" s="55">
+      <c r="C11" s="101"/>
+      <c r="D11" s="64">
         <v>2</v>
       </c>
       <c r="G11" s="18">
@@ -2976,16 +2963,16 @@
         <v>33</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>33</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="N11" s="21" t="s">
         <v>33</v>
@@ -2997,14 +2984,14 @@
         <v>33</v>
       </c>
       <c r="Q11" s="72" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="R11" s="73"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B12" s="58"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="55"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="64"/>
       <c r="G12" s="22">
         <v>5</v>
       </c>
@@ -3015,16 +3002,16 @@
         <v>33</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K12" s="32" t="s">
         <v>33</v>
       </c>
       <c r="L12" s="32" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="M12" s="32" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="N12" s="32" t="s">
         <v>33</v>
@@ -3035,22 +3022,22 @@
       <c r="P12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="Q12" s="92" t="s">
-        <v>95</v>
-      </c>
-      <c r="R12" s="93"/>
+      <c r="Q12" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="R12" s="95"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B13" s="57">
+      <c r="B13" s="65">
         <v>4</v>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="127">
+      <c r="C13" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="90">
         <v>1969</v>
       </c>
-      <c r="G13" s="130">
+      <c r="G13" s="53">
         <v>6</v>
       </c>
       <c r="H13" s="16"/>
@@ -3062,13 +3049,13 @@
       <c r="N13" s="33"/>
       <c r="O13" s="33"/>
       <c r="P13" s="33"/>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="93"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="95"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="128"/>
+      <c r="B14" s="93"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="91"/>
       <c r="G14" s="22">
         <v>7</v>
       </c>
@@ -3081,13 +3068,13 @@
       <c r="N14" s="33"/>
       <c r="O14" s="33"/>
       <c r="P14" s="33"/>
-      <c r="Q14" s="92"/>
-      <c r="R14" s="93"/>
+      <c r="Q14" s="94"/>
+      <c r="R14" s="95"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B15" s="83"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="129"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="92"/>
       <c r="G15" s="22">
         <v>8</v>
       </c>
@@ -3100,15 +3087,15 @@
       <c r="N15" s="33"/>
       <c r="O15" s="33"/>
       <c r="P15" s="33"/>
-      <c r="Q15" s="92"/>
-      <c r="R15" s="93"/>
+      <c r="Q15" s="94"/>
+      <c r="R15" s="95"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B16" s="83">
+      <c r="B16" s="93">
         <v>5</v>
       </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="127">
+      <c r="C16" s="93"/>
+      <c r="D16" s="90">
         <v>1970</v>
       </c>
       <c r="G16" s="22">
@@ -3123,13 +3110,13 @@
       <c r="N16" s="33"/>
       <c r="O16" s="33"/>
       <c r="P16" s="33"/>
-      <c r="Q16" s="92"/>
-      <c r="R16" s="93"/>
+      <c r="Q16" s="94"/>
+      <c r="R16" s="95"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B17" s="83"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="128"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="91"/>
       <c r="G17" s="22">
         <v>10</v>
       </c>
@@ -3142,13 +3129,13 @@
       <c r="N17" s="33"/>
       <c r="O17" s="33"/>
       <c r="P17" s="33"/>
-      <c r="Q17" s="92"/>
-      <c r="R17" s="93"/>
+      <c r="Q17" s="94"/>
+      <c r="R17" s="95"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="129"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="92"/>
       <c r="G18" s="22">
         <v>11</v>
       </c>
@@ -3161,14 +3148,14 @@
       <c r="N18" s="33"/>
       <c r="O18" s="33"/>
       <c r="P18" s="33"/>
-      <c r="Q18" s="92"/>
-      <c r="R18" s="93"/>
+      <c r="Q18" s="94"/>
+      <c r="R18" s="95"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B19" s="57">
+      <c r="B19" s="65">
         <v>23123</v>
       </c>
-      <c r="C19" s="84"/>
+      <c r="C19" s="100"/>
       <c r="D19" s="2"/>
       <c r="G19" s="22">
         <v>12</v>
@@ -3182,12 +3169,12 @@
       <c r="N19" s="33"/>
       <c r="O19" s="33"/>
       <c r="P19" s="33"/>
-      <c r="Q19" s="92"/>
-      <c r="R19" s="93"/>
+      <c r="Q19" s="94"/>
+      <c r="R19" s="95"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B20" s="83"/>
-      <c r="C20" s="85"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="101"/>
       <c r="D20" s="2"/>
       <c r="G20" s="22">
         <v>13</v>
@@ -3201,12 +3188,12 @@
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
       <c r="P20" s="33"/>
-      <c r="Q20" s="92"/>
-      <c r="R20" s="93"/>
+      <c r="Q20" s="94"/>
+      <c r="R20" s="95"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B21" s="83"/>
-      <c r="C21" s="85"/>
+      <c r="B21" s="93"/>
+      <c r="C21" s="101"/>
       <c r="D21" s="2"/>
       <c r="G21" s="22">
         <v>14</v>
@@ -3220,12 +3207,12 @@
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
       <c r="P21" s="33"/>
-      <c r="Q21" s="92"/>
-      <c r="R21" s="93"/>
+      <c r="Q21" s="94"/>
+      <c r="R21" s="95"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B22" s="83"/>
-      <c r="C22" s="85"/>
+      <c r="B22" s="93"/>
+      <c r="C22" s="101"/>
       <c r="D22" s="2"/>
       <c r="G22" s="22">
         <v>15</v>
@@ -3239,12 +3226,12 @@
       <c r="N22" s="33"/>
       <c r="O22" s="33"/>
       <c r="P22" s="33"/>
-      <c r="Q22" s="92"/>
-      <c r="R22" s="93"/>
+      <c r="Q22" s="94"/>
+      <c r="R22" s="95"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B23" s="83"/>
-      <c r="C23" s="85"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="101"/>
       <c r="D23" s="2"/>
       <c r="G23" s="22">
         <v>16</v>
@@ -3258,12 +3245,12 @@
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
       <c r="P23" s="33"/>
-      <c r="Q23" s="92"/>
-      <c r="R23" s="93"/>
+      <c r="Q23" s="94"/>
+      <c r="R23" s="95"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B24" s="58"/>
-      <c r="C24" s="86"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="102"/>
       <c r="D24" s="2"/>
       <c r="G24" s="22">
         <v>17</v>
@@ -3277,14 +3264,14 @@
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
       <c r="P24" s="33"/>
-      <c r="Q24" s="92"/>
-      <c r="R24" s="93"/>
+      <c r="Q24" s="94"/>
+      <c r="R24" s="95"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B25" s="57">
+      <c r="B25" s="65">
         <v>312312</v>
       </c>
-      <c r="C25" s="84" t="s">
+      <c r="C25" s="100" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -3302,77 +3289,74 @@
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
-      <c r="Q25" s="92"/>
-      <c r="R25" s="93"/>
+      <c r="Q25" s="94"/>
+      <c r="R25" s="95"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B26" s="83"/>
-      <c r="C26" s="85"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="101"/>
       <c r="D26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B27" s="83"/>
-      <c r="C27" s="85"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="101"/>
       <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B28" s="83"/>
-      <c r="C28" s="85"/>
+      <c r="B28" s="93"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="82"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="88"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="96"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="96"/>
       <c r="N28" s="41"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B29" s="83"/>
-      <c r="C29" s="85"/>
+      <c r="B29" s="93"/>
+      <c r="C29" s="101"/>
       <c r="D29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="103"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="103"/>
       <c r="N29" s="42"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B30" s="58"/>
-      <c r="C30" s="86"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="102"/>
       <c r="D30" s="2" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="C25:C30"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="Q7:R7"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:M28"/>
     <mergeCell ref="B5:D5"/>
@@ -3389,20 +3373,23 @@
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="Q8:R8"/>
     <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="C25:C30"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3418,7 +3405,7 @@
   <dimension ref="B1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3438,123 +3425,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="133" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B4" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="64" t="s">
+      <c r="C4" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="D4" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="E4" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="76" t="s">
+      <c r="F4" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="80" t="s">
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="80"/>
+      <c r="N4" s="78"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="101"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="94"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="130"/>
       <c r="F5" s="25" t="s">
         <v>30</v>
       </c>
       <c r="G5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="K5" s="129" t="s">
         <v>75</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" s="137" t="s">
-        <v>78</v>
-      </c>
-      <c r="L5" s="102"/>
+      <c r="L5" s="118"/>
       <c r="M5" s="25" t="s">
         <v>31</v>
       </c>
       <c r="N5" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B6" s="23">
         <v>1</v>
       </c>
-      <c r="C6" s="99" t="s">
-        <v>51</v>
+      <c r="C6" s="115" t="s">
+        <v>50</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="124" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="124" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" s="124" t="b">
+        <v>76</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="124">
+      <c r="J6" s="2">
         <v>3</v>
       </c>
-      <c r="K6" s="138" t="b">
+      <c r="K6" s="104" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="139"/>
+      <c r="L6" s="105"/>
       <c r="M6" s="28" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
@@ -3562,35 +3549,35 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="99"/>
+      <c r="C7" s="115"/>
       <c r="D7" s="30" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="124" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" s="124" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="124" t="s">
+      <c r="G7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="124" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="139"/>
+      <c r="J7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="105"/>
       <c r="M7" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
@@ -3598,19 +3585,19 @@
         <f t="shared" ref="B8:B12" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="99"/>
+      <c r="C8" s="115"/>
       <c r="D8" s="30" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="124" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="124" t="s">
-        <v>81</v>
+      <c r="G8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>33</v>
@@ -3618,15 +3605,15 @@
       <c r="J8" s="13">
         <v>2</v>
       </c>
-      <c r="K8" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="139"/>
+      <c r="K8" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="105"/>
       <c r="M8" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
@@ -3634,9 +3621,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="99"/>
+      <c r="C9" s="115"/>
       <c r="D9" s="30" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11" t="s">
@@ -3654,15 +3641,15 @@
       <c r="J9" s="13">
         <v>-12</v>
       </c>
-      <c r="K9" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="139"/>
+      <c r="K9" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="105"/>
       <c r="M9" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
@@ -3670,19 +3657,19 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="99"/>
+      <c r="C10" s="115"/>
       <c r="D10" s="30"/>
       <c r="E10" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>33</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I10" s="17" t="b">
         <v>1</v>
@@ -3690,15 +3677,15 @@
       <c r="J10" s="17">
         <v>0</v>
       </c>
-      <c r="K10" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="L10" s="139"/>
+      <c r="K10" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="105"/>
       <c r="M10" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
@@ -3706,10 +3693,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="99"/>
+      <c r="C11" s="115"/>
       <c r="D11" s="30"/>
       <c r="E11" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>33</v>
@@ -3726,15 +3713,15 @@
       <c r="J11" s="33">
         <v>1</v>
       </c>
-      <c r="K11" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" s="139"/>
+      <c r="K11" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="105"/>
       <c r="M11" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
@@ -3742,10 +3729,10 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="99"/>
+      <c r="C12" s="115"/>
       <c r="D12" s="30"/>
       <c r="E12" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>33</v>
@@ -3762,34 +3749,34 @@
       <c r="J12" s="33">
         <v>2</v>
       </c>
-      <c r="K12" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="L12" s="139"/>
+      <c r="K12" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="105"/>
       <c r="M12" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" s="123" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="131">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="54">
         <v>8</v>
       </c>
-      <c r="C13" s="99"/>
+      <c r="C13" s="115"/>
       <c r="D13" s="50"/>
-      <c r="E13" s="131" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="132" t="s">
+      <c r="E13" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="55" t="s">
         <v>34</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I13" s="21" t="s">
         <v>33</v>
@@ -3797,34 +3784,34 @@
       <c r="J13" s="17">
         <v>1</v>
       </c>
-      <c r="K13" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="L13" s="139"/>
-      <c r="M13" s="133" t="s">
-        <v>94</v>
-      </c>
-      <c r="N13" s="133" t="s">
-        <v>94</v>
+      <c r="K13" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="105"/>
+      <c r="M13" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" s="56" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="24">
         <v>9</v>
       </c>
-      <c r="C14" s="100"/>
+      <c r="C14" s="116"/>
       <c r="D14" s="31"/>
       <c r="E14" s="24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>33</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I14" s="32" t="s">
         <v>33</v>
@@ -3832,15 +3819,15 @@
       <c r="J14" s="33">
         <v>1</v>
       </c>
-      <c r="K14" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="139"/>
+      <c r="K14" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="105"/>
       <c r="M14" s="24" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N14" s="24" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -3860,7 +3847,7 @@
     </row>
     <row r="16" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="27"/>
@@ -3870,102 +3857,102 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="114"/>
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="110" t="s">
+      <c r="C18" s="108" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="37" t="s">
+      <c r="H18" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="110" t="s">
+      <c r="I18" s="109"/>
+      <c r="J18" s="110"/>
+      <c r="K18" s="110"/>
+      <c r="L18" s="111"/>
+      <c r="M18" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="113"/>
-      <c r="J18" s="111"/>
-      <c r="K18" s="111"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="110" t="s">
+      <c r="N18" s="109"/>
+      <c r="O18" s="110"/>
+      <c r="P18" s="111"/>
+    </row>
+    <row r="19" spans="2:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="122" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="113"/>
-      <c r="O18" s="111"/>
-      <c r="P18" s="112"/>
-    </row>
-    <row r="19" spans="2:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="106" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="107" t="s">
+      <c r="D19" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="108" t="s">
+      <c r="E19" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="108" t="s">
+      <c r="F19" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="109" t="s">
+      <c r="G19" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="118" t="s">
+      <c r="H19" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="114" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="115"/>
-      <c r="J19" s="108" t="s">
+      <c r="I19" s="125"/>
+      <c r="J19" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="108" t="s">
+      <c r="L19" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="L19" s="109" t="s">
-        <v>59</v>
-      </c>
-      <c r="M19" s="119" t="s">
-        <v>62</v>
-      </c>
-      <c r="N19" s="108" t="s">
+      <c r="M19" s="112" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="O19" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="O19" s="108" t="s">
+      <c r="P19" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="P19" s="109" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B20" s="106"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="108"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="109"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="108"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="120"/>
-      <c r="N20" s="108"/>
-      <c r="O20" s="108"/>
-      <c r="P20" s="109"/>
+      <c r="B20" s="122"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="126"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="107"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="106"/>
+      <c r="M20" s="113"/>
+      <c r="N20" s="107"/>
+      <c r="O20" s="107"/>
+      <c r="P20" s="106"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="36">
         <v>8</v>
@@ -3980,10 +3967,10 @@
       <c r="G21" s="44">
         <v>4</v>
       </c>
-      <c r="H21" s="104" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" s="105"/>
+      <c r="H21" s="120" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" s="121"/>
       <c r="J21" s="2">
         <v>4</v>
       </c>
@@ -3994,13 +3981,13 @@
         <v>0</v>
       </c>
       <c r="M21" s="43" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="N21" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O21" s="38">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P21" s="39">
         <v>0</v>
@@ -4011,29 +3998,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C6:C14"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="K19:K20"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="M4:N4"/>
@@ -4049,6 +4013,29 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="K8:L8"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4057,6 +4044,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -4200,22 +4202,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33EFF49E-866D-4BFD-B7FD-9BB436667B53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4231,21 +4235,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>